<commit_message>
Updated info files and added header info in factor_info.xlsx
</commit_message>
<xml_diff>
--- a/NKI/factor_info.xlsx
+++ b/NKI/factor_info.xlsx
@@ -1,31 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaitanya/Documents/Research/SequenceEngineering/NKI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaitanya/Documents/GitWorkspaces/NKICollab/NKI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A37FE2FB-A2C4-6E46-845A-91510F9AAEBE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6FA2F7-4563-6B49-A7E6-D39DC85A8DDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6900" yWindow="5040" windowWidth="27240" windowHeight="16440" xr2:uid="{5BF7AA58-BE2C-5044-9B9B-4C274D2B6324}"/>
+    <workbookView xWindow="700" yWindow="1360" windowWidth="27240" windowHeight="16440" xr2:uid="{5BF7AA58-BE2C-5044-9B9B-4C274D2B6324}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="117">
   <si>
     <t>TF</t>
   </si>
@@ -1103,13 +1113,43 @@
   </si>
   <si>
     <t>Poor motifs that disagree</t>
+  </si>
+  <si>
+    <t>Legend:</t>
+  </si>
+  <si>
+    <t>Transcription factor name from mt20191119_TFs_list_updated</t>
+  </si>
+  <si>
+    <t>Motif from mt20191119_TFs_list_updated</t>
+  </si>
+  <si>
+    <t>The two positions mutated in order to kill binding, as decided by Chaitanya</t>
+  </si>
+  <si>
+    <t>The source motif used to guide modification selection/decision</t>
+  </si>
+  <si>
+    <t>Is a ProBound model missing for this factor? (note, this is circa Nov 2019)</t>
+  </si>
+  <si>
+    <t>* Please note, Smad1 was ignored for some reason.</t>
+  </si>
+  <si>
+    <t>Is SELEX info used to make a decision on the motif?</t>
+  </si>
+  <si>
+    <t>Is a mouse-based TF Motif being used to guide sequence decisions?</t>
+  </si>
+  <si>
+    <t>Wether or not data + motif exist for this factor, as of Nov 2019</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1128,6 +1168,14 @@
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri (Body)_x0000_"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1150,25 +1198,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1499,10 +1541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2062675-2DAA-B049-A192-3E20DB77BBF9}">
-  <dimension ref="A1:N31"/>
+  <dimension ref="A1:N45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection activeCell="B33" sqref="B33:B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1592,10 +1634,10 @@
         <f>OR(B2="Yes",C2="Yes")</f>
         <v>0</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="1" t="s">
         <v>68</v>
       </c>
       <c r="L2" t="s">
@@ -1632,10 +1674,10 @@
         <f t="shared" ref="I3:I28" si="1">OR(B3="Yes",C3="Yes")</f>
         <v>0</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="1" t="s">
         <v>69</v>
       </c>
       <c r="L3" t="s">
@@ -1672,10 +1714,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="1" t="s">
         <v>70</v>
       </c>
       <c r="L4" t="s">
@@ -1712,7 +1754,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1746,7 +1788,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J6" s="1" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1780,10 +1822,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="K7" s="1" t="s">
         <v>71</v>
       </c>
       <c r="L7" t="s">
@@ -1820,10 +1862,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="K8" s="1" t="s">
         <v>75</v>
       </c>
       <c r="L8" t="s">
@@ -1863,10 +1905,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="K9" s="1" t="s">
         <v>77</v>
       </c>
       <c r="L9" t="s">
@@ -1906,10 +1948,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="K10" s="1" t="s">
         <v>78</v>
       </c>
       <c r="L10" t="s">
@@ -1917,7 +1959,7 @@
       </c>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" t="s">
@@ -1946,10 +1988,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="J11" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="K11" s="1" t="s">
         <v>79</v>
       </c>
       <c r="L11" t="s">
@@ -1960,7 +2002,7 @@
       </c>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" t="s">
@@ -1989,10 +2031,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="J12" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="K12" s="1" t="s">
         <v>99</v>
       </c>
       <c r="L12" t="s">
@@ -2000,7 +2042,7 @@
       </c>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13" t="s">
@@ -2029,10 +2071,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J13" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="K13" s="1" t="s">
         <v>98</v>
       </c>
       <c r="L13" t="s">
@@ -2040,7 +2082,7 @@
       </c>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14" t="s">
@@ -2069,10 +2111,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="J14" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="K14" s="1" t="s">
         <v>105</v>
       </c>
       <c r="L14" t="s">
@@ -2083,7 +2125,7 @@
       </c>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15" t="s">
@@ -2112,10 +2154,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="J15" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="K15" s="1" t="s">
         <v>101</v>
       </c>
       <c r="L15" t="s">
@@ -2123,7 +2165,7 @@
       </c>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16" t="s">
@@ -2152,10 +2194,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="J16" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="K16" s="1" t="s">
         <v>89</v>
       </c>
       <c r="L16" t="s">
@@ -2163,7 +2205,7 @@
       </c>
     </row>
     <row r="17" spans="1:14">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17" t="s">
@@ -2192,10 +2234,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="J17" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="K17" s="2" t="s">
+      <c r="K17" s="1" t="s">
         <v>103</v>
       </c>
       <c r="L17" t="s">
@@ -2209,7 +2251,7 @@
       </c>
     </row>
     <row r="18" spans="1:14">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="B18" t="s">
@@ -2238,7 +2280,7 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="J18" s="1" t="s">
         <v>55</v>
       </c>
       <c r="K18" t="s">
@@ -2249,7 +2291,7 @@
       </c>
     </row>
     <row r="19" spans="1:14">
-      <c r="A19" s="1" t="s">
+      <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19" t="s">
@@ -2278,10 +2320,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="J19" s="2" t="s">
+      <c r="J19" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="K19" s="2" t="s">
+      <c r="K19" s="1" t="s">
         <v>96</v>
       </c>
       <c r="L19" t="s">
@@ -2292,7 +2334,7 @@
       </c>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="1" t="s">
+      <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20" t="s">
@@ -2321,10 +2363,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="J20" s="2" t="s">
+      <c r="J20" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K20" s="2" t="s">
+      <c r="K20" s="1" t="s">
         <v>92</v>
       </c>
       <c r="L20" t="s">
@@ -2361,10 +2403,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="J21" s="2" t="s">
+      <c r="J21" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K21" s="2" t="s">
+      <c r="K21" s="1" t="s">
         <v>104</v>
       </c>
       <c r="L21" t="s">
@@ -2375,7 +2417,7 @@
       </c>
     </row>
     <row r="22" spans="1:14">
-      <c r="A22" s="1" t="s">
+      <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22" t="s">
@@ -2404,10 +2446,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="J22" s="2" t="s">
+      <c r="J22" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="K22" s="2" t="s">
+      <c r="K22" s="1" t="s">
         <v>91</v>
       </c>
       <c r="L22" t="s">
@@ -2415,7 +2457,7 @@
       </c>
     </row>
     <row r="23" spans="1:14">
-      <c r="A23" s="1" t="s">
+      <c r="A23" t="s">
         <v>23</v>
       </c>
       <c r="B23" t="s">
@@ -2444,10 +2486,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J23" s="2" t="s">
+      <c r="J23" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="K23" s="2" t="s">
+      <c r="K23" s="1" t="s">
         <v>100</v>
       </c>
       <c r="L23" t="s">
@@ -2484,10 +2526,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="J24" s="2" t="s">
+      <c r="J24" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="K24" s="2" t="s">
+      <c r="K24" s="1" t="s">
         <v>88</v>
       </c>
       <c r="L24" t="s">
@@ -2524,10 +2566,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="J25" s="2" t="s">
+      <c r="J25" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="K25" s="2" t="s">
+      <c r="K25" s="1" t="s">
         <v>85</v>
       </c>
       <c r="L25" t="s">
@@ -2535,7 +2577,7 @@
       </c>
     </row>
     <row r="26" spans="1:14">
-      <c r="A26" s="1" t="s">
+      <c r="A26" t="s">
         <v>26</v>
       </c>
       <c r="B26" t="s">
@@ -2564,10 +2606,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="J26" s="2" t="s">
+      <c r="J26" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K26" s="2" t="s">
+      <c r="K26" s="1" t="s">
         <v>82</v>
       </c>
       <c r="L26" t="s">
@@ -2575,7 +2617,7 @@
       </c>
     </row>
     <row r="27" spans="1:14">
-      <c r="A27" s="1" t="s">
+      <c r="A27" t="s">
         <v>27</v>
       </c>
       <c r="B27" t="s">
@@ -2604,10 +2646,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="J27" s="2" t="s">
+      <c r="J27" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K27" s="2" t="s">
+      <c r="K27" s="1" t="s">
         <v>81</v>
       </c>
       <c r="L27" t="s">
@@ -2618,7 +2660,7 @@
       </c>
     </row>
     <row r="28" spans="1:14">
-      <c r="A28" s="1" t="s">
+      <c r="A28" t="s">
         <v>28</v>
       </c>
       <c r="B28" t="s">
@@ -2647,10 +2689,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="J28" s="2" t="s">
+      <c r="J28" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="K28" s="2" t="s">
+      <c r="K28" s="1" t="s">
         <v>80</v>
       </c>
       <c r="L28" t="s">
@@ -2658,20 +2700,120 @@
       </c>
     </row>
     <row r="31" spans="1:14">
-      <c r="K31" s="2"/>
+      <c r="A31" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="K31" s="1"/>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="4"/>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" s="4"/>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" s="4"/>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37" s="4"/>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" s="4"/>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B39" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>65</v>
+      </c>
+      <c r="B42" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>66</v>
+      </c>
+      <c r="B43" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>74</v>
+      </c>
+      <c r="B44" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>113</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B33:B38"/>
+  </mergeCells>
   <conditionalFormatting sqref="B2:G28">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H28">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I28">
+  <conditionalFormatting sqref="H2:I28">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>FALSE</formula>
     </cfRule>

</xml_diff>